<commit_message>
Function for Projects Page
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginHRM.xlsx
+++ b/src/test/resources/testdata/LoginHRM.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Java\Project\FinalProjectAutomationTest\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A53F62-4FC3-4F0D-8E2B-AA292CD3798F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281F96E5-AE00-4B66-B06A-8511252E5564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="1845" windowWidth="23985" windowHeight="13470" xr2:uid="{79BA1FD9-04F7-446D-A190-015AACA01288}"/>
+    <workbookView xWindow="705" yWindow="3345" windowWidth="23985" windowHeight="13470" activeTab="3" xr2:uid="{79BA1FD9-04F7-446D-A190-015AACA01288}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Clients" sheetId="2" r:id="rId2"/>
+    <sheet name="Projects" sheetId="3" r:id="rId3"/>
+    <sheet name="Tasks" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Login!$C:$C</definedName>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
   <si>
     <t>USERNAME</t>
   </si>
@@ -282,6 +284,39 @@
   </si>
   <si>
     <t>Passrowd@12</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>CLIENT</t>
+  </si>
+  <si>
+    <t>HOUR</t>
+  </si>
+  <si>
+    <t>PRIORITY</t>
+  </si>
+  <si>
+    <t>START_DATE</t>
+  </si>
+  <si>
+    <t>END_DATE</t>
+  </si>
+  <si>
+    <t>SUMMARY</t>
+  </si>
+  <si>
+    <t>TEAM</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>PROJECT</t>
+  </si>
+  <si>
+    <t>ATTACH</t>
   </si>
 </sst>
 </file>
@@ -656,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367340E2-5DAD-4A3F-9862-8048D7AC0F7E}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:K1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +702,7 @@
     <col min="5" max="5" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1091,4 +1126,92 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69497AEC-9A82-4E0A-918B-D939B39B005B}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE938AD-32A7-4EED-A9B8-EE1C285E7213}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Task and Status
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginHRM.xlsx
+++ b/src/test/resources/testdata/LoginHRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Java\Project\FinalProjectAutomationTest\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281F96E5-AE00-4B66-B06A-8511252E5564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE330D6-2188-4030-A8F1-F65388A0635C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="3345" windowWidth="23985" windowHeight="13470" activeTab="3" xr2:uid="{79BA1FD9-04F7-446D-A190-015AACA01288}"/>
+    <workbookView xWindow="3945" yWindow="6960" windowWidth="21375" windowHeight="13470" activeTab="2" xr2:uid="{79BA1FD9-04F7-446D-A190-015AACA01288}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="159">
   <si>
     <t>USERNAME</t>
   </si>
@@ -317,12 +317,237 @@
   </si>
   <si>
     <t>ATTACH</t>
+  </si>
+  <si>
+    <t>Project A</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Building the application</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Designing the user interface</t>
+  </si>
+  <si>
+    <t>Project C</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Testing the application</t>
+  </si>
+  <si>
+    <t>Project D</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Analyzing data and results</t>
+  </si>
+  <si>
+    <t>Project E</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>Deploying the application</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Performing routine maintenance</t>
+  </si>
+  <si>
+    <t>Project B</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Admin Example</t>
+  </si>
+  <si>
+    <t>Task 1</t>
+  </si>
+  <si>
+    <t>Initial Setup</t>
+  </si>
+  <si>
+    <t>Setting up project infrastructure</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Task 2</t>
+  </si>
+  <si>
+    <t>Data Collection</t>
+  </si>
+  <si>
+    <t>Gathering data for analysis</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Task 3</t>
+  </si>
+  <si>
+    <t>Task 4</t>
+  </si>
+  <si>
+    <t>Task 5</t>
+  </si>
+  <si>
+    <t>Task 6</t>
+  </si>
+  <si>
+    <t>Task 7</t>
+  </si>
+  <si>
+    <t>Task 8</t>
+  </si>
+  <si>
+    <t>Reporting</t>
+  </si>
+  <si>
+    <t>Creating reports and summaries</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>On Hold</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Jan, 2024, 01</t>
+  </si>
+  <si>
+    <t>May, 2024, 05</t>
+  </si>
+  <si>
+    <t>Aug, 2024, 10</t>
+  </si>
+  <si>
+    <t>Mar, 2024, 15</t>
+  </si>
+  <si>
+    <t>Jan, 2024, 20</t>
+  </si>
+  <si>
+    <t>Jan, 2025, 10</t>
+  </si>
+  <si>
+    <t>Jun, 2025, 15</t>
+  </si>
+  <si>
+    <t>Oct, 2025, 25</t>
+  </si>
+  <si>
+    <t>Jun, 2025, 25</t>
+  </si>
+  <si>
+    <t>Feb, 2025, 05</t>
+  </si>
+  <si>
+    <t>Feb, 2024, 01</t>
+  </si>
+  <si>
+    <t>Aug, 2024, 13</t>
+  </si>
+  <si>
+    <t>Jun, 2024, 03</t>
+  </si>
+  <si>
+    <t>Nov, 2024, 07</t>
+  </si>
+  <si>
+    <t>Jul, 2024, 10</t>
+  </si>
+  <si>
+    <t>Aug, 2024, 12</t>
+  </si>
+  <si>
+    <t>Feb, 2024, 03</t>
+  </si>
+  <si>
+    <t>Jan, 2024, 05</t>
+  </si>
+  <si>
+    <t>Sep, 2024, 07</t>
+  </si>
+  <si>
+    <t>Dec, 2024, 10</t>
+  </si>
+  <si>
+    <t>Jul, 2024, 15</t>
+  </si>
+  <si>
+    <t>Oct, 2024, 15</t>
+  </si>
+  <si>
+    <t>Mar, 2024, 18</t>
+  </si>
+  <si>
+    <t>Jan, 2024, 18</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Highest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]mmm\,\ yyyy\,\ dd"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,12 +572,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -360,11 +585,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,9 +612,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,7 +942,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:XFD1048576"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,19 +953,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>71</v>
       </c>
     </row>
@@ -817,7 +1067,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:R1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,57 +1090,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
@@ -934,10 +1184,10 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
@@ -981,10 +1231,10 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C4" t="s">
@@ -1028,10 +1278,10 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>48</v>
       </c>
       <c r="C5" t="s">
@@ -1075,10 +1325,10 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C6" t="s">
@@ -1130,88 +1380,460 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69497AEC-9A82-4E0A-918B-D939B39B005B}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="9" t="s">
         <v>82</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="8" t="str">
+        <f>_xlfn.CONCAT(Clients!A2, " ",Clients!B2)</f>
+        <v>John Doe</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="8" t="str">
+        <f>_xlfn.CONCAT(Clients!A3, " ",Clients!B3)</f>
+        <v>Jane Doe</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="8" t="str">
+        <f>_xlfn.CONCAT(Clients!A4, " ",Clients!B4)</f>
+        <v>Bob Smith</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="8" t="str">
+        <f>_xlfn.CONCAT(Clients!A5, " ",Clients!B5)</f>
+        <v>Alice Johnson</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="8" t="str">
+        <f>_xlfn.CONCAT(Clients!A6, " ",Clients!B6)</f>
+        <v>Mike Brown</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE938AD-32A7-4EED-A9B8-EE1C285E7213}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="14.7109375" style="5"/>
+    <col min="7" max="7" width="22.28515625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="14.7109375" style="5"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="10" t="s">
         <v>84</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All Function in Project
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginHRM.xlsx
+++ b/src/test/resources/testdata/LoginHRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Java\Project\FinalProjectAutomationTest\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE330D6-2188-4030-A8F1-F65388A0635C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7CD3C9-C3EE-4BE3-B09C-1C6A102B1CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="6960" windowWidth="21375" windowHeight="13470" activeTab="2" xr2:uid="{79BA1FD9-04F7-446D-A190-015AACA01288}"/>
+    <workbookView xWindow="2385" yWindow="1785" windowWidth="23640" windowHeight="13470" activeTab="1" xr2:uid="{79BA1FD9-04F7-446D-A190-015AACA01288}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="166">
   <si>
     <t>USERNAME</t>
   </si>
@@ -370,9 +370,6 @@
     <t>Maintenance</t>
   </si>
   <si>
-    <t>Performing routine maintenance</t>
-  </si>
-  <si>
     <t>Project B</t>
   </si>
   <si>
@@ -388,9 +385,6 @@
     <t>Initial Setup</t>
   </si>
   <si>
-    <t>Setting up project infrastructure</t>
-  </si>
-  <si>
     <t>In Progress</t>
   </si>
   <si>
@@ -400,9 +394,6 @@
     <t>Data Collection</t>
   </si>
   <si>
-    <t>Gathering data for analysis</t>
-  </si>
-  <si>
     <t>Not Started</t>
   </si>
   <si>
@@ -427,9 +418,6 @@
     <t>Reporting</t>
   </si>
   <si>
-    <t>Creating reports and summaries</t>
-  </si>
-  <si>
     <t>Cancelled</t>
   </si>
   <si>
@@ -539,6 +527,39 @@
   </si>
   <si>
     <t>Highest</t>
+  </si>
+  <si>
+    <t>Setting up project infrastructure: This involves configuring servers, databases, and networks to support the project's software development and deployment needs.</t>
+  </si>
+  <si>
+    <t>Deploying the application: This involves configuring servers, databases, and networks to support the project's software development and deployment needs.</t>
+  </si>
+  <si>
+    <t>Gathering data for analysis: This involves configuring servers, databases, and networks to support the project's software development and deployment needs.</t>
+  </si>
+  <si>
+    <t>Performing routine maintenance: This involves configuring servers, databases, and networks to support the project's software development and deployment needs.</t>
+  </si>
+  <si>
+    <t>Building the application: It encompasses writing code, integrating modules, and following design specifications to create a functional software product or system.</t>
+  </si>
+  <si>
+    <t>Testing the application: This process involves executing various test cases, including unit, integration, and acceptance tests, to validate functionality, performance, and user experience.</t>
+  </si>
+  <si>
+    <t>Analyzing data and results: It involves applying statistical methods, machine learning algorithms, or other analytical techniques to interpret data and draw meaningful conclusions.</t>
+  </si>
+  <si>
+    <t>Creating reports and summaries: This task includes synthesizing findings, visualizing data, and presenting actionable insights in reports or presentations tailored to stakeholders' needs.</t>
+  </si>
+  <si>
+    <t>/src/test/resources/testdata/Task.png</t>
+  </si>
+  <si>
+    <t>TITLE_FILE</t>
+  </si>
+  <si>
+    <t>TestFile</t>
   </si>
 </sst>
 </file>
@@ -977,21 +998,21 @@
         <v>3</v>
       </c>
       <c r="C2" t="str" cm="1">
-        <f t="array" ref="C2">IF(Clients!$H2 = "Active", "Active", null)</f>
+        <f t="array" ref="C2">IF(Clients!$H3 = "Active", "Active", null)</f>
         <v>Active</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="str" cm="1">
-        <f t="array" ref="A3">IF($C$2=Clients!$H2,Clients!G2, null)</f>
+        <f t="array" ref="A3">IF($C$2=Clients!$H3,Clients!G3, null)</f>
         <v>johndoe</v>
       </c>
       <c r="B3" t="str" cm="1">
-        <f t="array" ref="B3">IF($C$2=Clients!$H2,Clients!C2, null)</f>
+        <f t="array" ref="B3">IF($C$2=Clients!$H3,Clients!C3, null)</f>
         <v>password123</v>
       </c>
       <c r="C3" t="str">
-        <f>IF($C$2=Clients!$H2,Clients!H2,Clients!$H$3)</f>
+        <f>IF($C$2=Clients!$H3,Clients!H3,Clients!$H$4)</f>
         <v>Active</v>
       </c>
       <c r="D3" t="s">
@@ -1003,57 +1024,57 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>IF($C$2=Clients!$H3,Clients!G3, Clients!G3)</f>
+        <f>IF($C$2=Clients!$H4,Clients!G4, Clients!G4)</f>
         <v>janedoe</v>
       </c>
       <c r="B4" t="str">
-        <f>IF($C$2=Clients!$H3,Clients!C3, Clients!C3)</f>
+        <f>IF($C$2=Clients!$H4,Clients!C4, Clients!C4)</f>
         <v>password123</v>
       </c>
       <c r="C4" t="str">
-        <f>IF($C$2=Clients!$H3,Clients!H3,Clients!$H$3)</f>
+        <f>IF($C$2=Clients!$H4,Clients!H4,Clients!$H$4)</f>
         <v>Banned</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>IF($C$2=Clients!$H4,Clients!G4, Clients!G4)</f>
+        <f>IF($C$2=Clients!$H5,Clients!G5, Clients!G5)</f>
         <v>bobsmith</v>
       </c>
       <c r="B5" t="str">
-        <f>IF($C$2=Clients!$H4,Clients!C4, Clients!C4)</f>
+        <f>IF($C$2=Clients!$H5,Clients!C5, Clients!C5)</f>
         <v>password123</v>
       </c>
       <c r="C5" t="str">
-        <f>IF($C$2=Clients!$H4,Clients!H4,Clients!$H$3)</f>
+        <f>IF($C$2=Clients!$H5,Clients!H5,Clients!$H$4)</f>
         <v>Active</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>IF($C$2=Clients!$H5,Clients!G5, Clients!G5)</f>
+        <f>IF($C$2=Clients!$H6,Clients!G6, Clients!G6)</f>
         <v>alicejohnson</v>
       </c>
       <c r="B6" t="str">
-        <f>IF($C$2=Clients!$H5,Clients!C5, Clients!C5)</f>
+        <f>IF($C$2=Clients!$H6,Clients!C6, Clients!C6)</f>
         <v>password123</v>
       </c>
       <c r="C6" t="str">
-        <f>IF($C$2=Clients!$H5,Clients!H5,Clients!$H$3)</f>
+        <f>IF($C$2=Clients!$H6,Clients!H6,Clients!$H$4)</f>
         <v>Banned</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="str" cm="1">
-        <f t="array" ref="A7">IF($C$2=Clients!$H6,Clients!G6, null)</f>
+        <f t="array" ref="A7">IF($C$2=Clients!$H7,Clients!G7, null)</f>
         <v>mikebrown</v>
       </c>
       <c r="B7" t="str">
-        <f>IF($C$2=Clients!$H6,Clients!C6, Clients!C6)</f>
+        <f>IF($C$2=Clients!$H7,Clients!C7, Clients!C7)</f>
         <v>password123</v>
       </c>
       <c r="C7" t="str">
-        <f>IF($C$2=Clients!$H6,Clients!H6,Clients!$H$3)</f>
+        <f>IF($C$2=Clients!$H7,Clients!H7,Clients!$H$4)</f>
         <v>Active</v>
       </c>
     </row>
@@ -1064,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278CEAAF-5CBB-47DB-8AF0-25EE750EE6FA}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,56 +1157,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2">
-        <v>10001</v>
-      </c>
-      <c r="O2" t="s">
-        <v>64</v>
-      </c>
-    </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
@@ -1194,37 +1168,37 @@
         <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="M3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="N3">
-        <v>90001</v>
+        <v>10001</v>
       </c>
       <c r="O3" t="s">
         <v>64</v>
@@ -1232,46 +1206,46 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="M4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N4">
-        <v>80202</v>
+        <v>90001</v>
       </c>
       <c r="O4" t="s">
         <v>64</v>
@@ -1279,46 +1253,46 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="J5" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="K5" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="L5" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="M5" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="N5">
-        <v>60606</v>
+        <v>80202</v>
       </c>
       <c r="O5" t="s">
         <v>64</v>
@@ -1326,48 +1300,95 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I6" t="s">
         <v>67</v>
       </c>
       <c r="J6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="M6" t="s">
         <v>69</v>
       </c>
       <c r="N6">
+        <v>60606</v>
+      </c>
+      <c r="O6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N7">
         <v>94105</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O7" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1380,10 +1401,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69497AEC-9A82-4E0A-918B-D939B39B005B}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,153 +1444,153 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="8" t="str">
-        <f>_xlfn.CONCAT(Clients!A2, " ",Clients!B2)</f>
-        <v>John Doe</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B3" s="8" t="str">
         <f>_xlfn.CONCAT(Clients!A3, " ",Clients!B3)</f>
-        <v>Jane Doe</v>
+        <v>John Doe</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="G3" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B4" s="8" t="str">
         <f>_xlfn.CONCAT(Clients!A4, " ",Clients!B4)</f>
-        <v>Bob Smith</v>
+        <v>Jane Doe</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E4" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>140</v>
-      </c>
       <c r="G4" s="8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B5" s="8" t="str">
         <f>_xlfn.CONCAT(Clients!A5, " ",Clients!B5)</f>
-        <v>Alice Johnson</v>
+        <v>Bob Smith</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="E5" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>141</v>
-      </c>
       <c r="G5" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>104</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B6" s="8" t="str">
         <f>_xlfn.CONCAT(Clients!A6, " ",Clients!B6)</f>
+        <v>Alice Johnson</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="8" t="str">
+        <f>_xlfn.CONCAT(Clients!A7, " ",Clients!B7)</f>
         <v>Mike Brown</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="C7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="I6" s="8" t="s">
+      <c r="H7" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1582,20 +1603,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE938AD-32A7-4EED-A9B8-EE1C285E7213}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L1048576"/>
+      <selection activeCell="M1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="6" width="14.7109375" style="5"/>
-    <col min="7" max="7" width="22.28515625" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="14.7109375" style="5"/>
+    <col min="7" max="7" width="35.7109375" style="5" customWidth="1"/>
+    <col min="8" max="9" width="14.7109375" style="5"/>
+    <col min="11" max="16384" width="14.7109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>74</v>
       </c>
@@ -1621,219 +1643,306 @@
         <v>10</v>
       </c>
       <c r="I1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="H3" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="5" t="str">
+        <f>(VLOOKUP(E3,Projects!A3:B7,2,1))</f>
+        <v>John Doe</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C4" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D4" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I4" s="5" t="str">
+        <f>(VLOOKUP(E4,Projects!A4:B7,2,1))</f>
+        <v>Jane Doe</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="5" t="str">
+        <f>(VLOOKUP(E5,Projects!A5:B7,2,1))</f>
+        <v>Bob Smith</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" s="5" t="str">
+        <f>(VLOOKUP(E6,Projects!A6:B7,2,1))</f>
+        <v>Alice Johnson</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="5" t="str">
+        <f>(VLOOKUP(E7,Projects!A3:B7,2,1))</f>
+        <v>Mike Brown</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="F8" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="I8" s="5" t="str">
+        <f>(VLOOKUP(E8,Projects!A3:B7,2,1))</f>
+        <v>John Doe</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="D9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="I9" s="5" t="str">
+        <f>(VLOOKUP(E9,Projects!A4:B7,2,1))</f>
+        <v>Jane Doe</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="F10" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>113</v>
+      <c r="H10" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" s="5" t="str">
+        <f>(VLOOKUP(E10,Projects!A5:B7,2,1))</f>
+        <v>Mike Brown</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Full Flow Manage Clients
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginHRM.xlsx
+++ b/src/test/resources/testdata/LoginHRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Java\Project\FinalProjectAutomationTest\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7CD3C9-C3EE-4BE3-B09C-1C6A102B1CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADD1C6F-AA5C-4FDB-9B36-2680FABE79D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="1785" windowWidth="23640" windowHeight="13470" activeTab="1" xr2:uid="{79BA1FD9-04F7-446D-A190-015AACA01288}"/>
+    <workbookView xWindow="885" yWindow="3195" windowWidth="19935" windowHeight="13470" activeTab="1" xr2:uid="{79BA1FD9-04F7-446D-A190-015AACA01288}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="260">
   <si>
     <t>USERNAME</t>
   </si>
@@ -560,6 +560,288 @@
   </si>
   <si>
     <t>TestFile</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>emily.wilson@example.com</t>
+  </si>
+  <si>
+    <t>emilywilson</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>1111 Bond St</t>
+  </si>
+  <si>
+    <t>Apt 606</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>NSW</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>david.lee@example.com</t>
+  </si>
+  <si>
+    <t>davidlee</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>2222 Raffles Ave</t>
+  </si>
+  <si>
+    <t>Apt 1001</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>sarah.taylor@example.com</t>
+  </si>
+  <si>
+    <t>sarahtaylor</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>3333 Champs Elysees</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>IDF</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>kevin.white@example.com</t>
+  </si>
+  <si>
+    <t>kevinwhite</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>4444 Berliner Str</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Project F</t>
+  </si>
+  <si>
+    <t>Emily Smith</t>
+  </si>
+  <si>
+    <t>Apr, 2024, 01</t>
+  </si>
+  <si>
+    <t>May, 2025, 15</t>
+  </si>
+  <si>
+    <t>Building the infrastructure</t>
+  </si>
+  <si>
+    <t>Project G</t>
+  </si>
+  <si>
+    <t>David Lee</t>
+  </si>
+  <si>
+    <t>Aug, 2025, 20</t>
+  </si>
+  <si>
+    <t>Designing the database schema</t>
+  </si>
+  <si>
+    <t>Project H</t>
+  </si>
+  <si>
+    <t>Sarah Taylor</t>
+  </si>
+  <si>
+    <t>Dec, 2025, 30</t>
+  </si>
+  <si>
+    <t>Testing the database</t>
+  </si>
+  <si>
+    <t>Project I</t>
+  </si>
+  <si>
+    <t>Kevin White</t>
+  </si>
+  <si>
+    <t>Mar, 2025, 25</t>
+  </si>
+  <si>
+    <t>Analyzing the code</t>
+  </si>
+  <si>
+    <t>Project J</t>
+  </si>
+  <si>
+    <t>Jessica Brown</t>
+  </si>
+  <si>
+    <t>Mar, 2025, 15</t>
+  </si>
+  <si>
+    <t>Deploying the code</t>
+  </si>
+  <si>
+    <t>Task 9</t>
+  </si>
+  <si>
+    <t>Feb, 2024, 20</t>
+  </si>
+  <si>
+    <t>Feb, 2024, 25</t>
+  </si>
+  <si>
+    <t>Designing the user interface: This involves creating wireframes, prototypes, and high-fidelity designs to visualize and interact with the application's user interface.</t>
+  </si>
+  <si>
+    <t>UI Design</t>
+  </si>
+  <si>
+    <t>Bob Smith</t>
+  </si>
+  <si>
+    <t>Task 10</t>
+  </si>
+  <si>
+    <t>Mar, 2024, 01</t>
+  </si>
+  <si>
+    <t>Mar, 2024, 05</t>
+  </si>
+  <si>
+    <t>Developing the database schema: This task involves designing and implementing the database structure, including tables, relationships, and indexes, to support the application's data storage needs.</t>
+  </si>
+  <si>
+    <t>Database Design</t>
+  </si>
+  <si>
+    <t>Alice Johnson</t>
+  </si>
+  <si>
+    <t>Task 11</t>
+  </si>
+  <si>
+    <t>Apr, 2024, 10</t>
+  </si>
+  <si>
+    <t>Apr, 2024, 15</t>
+  </si>
+  <si>
+    <t>Mike Brown</t>
+  </si>
+  <si>
+    <t>Task 12</t>
+  </si>
+  <si>
+    <t>May, 2024, 01</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>JaneDoe1</t>
+  </si>
+  <si>
+    <t>Passw0rd123</t>
+  </si>
+  <si>
+    <t>BobSmith1</t>
+  </si>
+  <si>
+    <t>P@ssw0rd123</t>
+  </si>
+  <si>
+    <t>AliceJ1</t>
+  </si>
+  <si>
+    <t>P@ssword123</t>
+  </si>
+  <si>
+    <t>MikeB1</t>
+  </si>
+  <si>
+    <t>MikeP@ss</t>
+  </si>
+  <si>
+    <t>EmilyW1</t>
+  </si>
+  <si>
+    <t>EwilsonP@ss</t>
+  </si>
+  <si>
+    <t>DavidL1</t>
+  </si>
+  <si>
+    <t>DleeP@ss123</t>
+  </si>
+  <si>
+    <t>SarahT1</t>
+  </si>
+  <si>
+    <t>STaylorP@ss</t>
+  </si>
+  <si>
+    <t>KevinW1</t>
+  </si>
+  <si>
+    <t>KevinP@ss123</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>5555551234</t>
+  </si>
+  <si>
+    <t>5556667890</t>
+  </si>
+  <si>
+    <t>5557771234</t>
+  </si>
+  <si>
+    <t>5558881234</t>
+  </si>
+  <si>
+    <t>Kevin</t>
   </si>
 </sst>
 </file>
@@ -625,7 +907,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -646,6 +928,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -960,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367340E2-5DAD-4A3F-9862-8048D7AC0F7E}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B31" sqref="B30:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,22 +1281,19 @@
         <v>3</v>
       </c>
       <c r="C2" t="str" cm="1">
-        <f t="array" ref="C2">IF(Clients!$H3 = "Active", "Active", null)</f>
+        <f t="array" ref="C2">IF(Clients!$H2 = "Active", "Active", null)</f>
         <v>Active</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="str" cm="1">
-        <f t="array" ref="A3">IF($C$2=Clients!$H3,Clients!G3, null)</f>
-        <v>johndoe</v>
-      </c>
-      <c r="B3" t="str" cm="1">
-        <f t="array" ref="B3">IF($C$2=Clients!$H3,Clients!C3, null)</f>
-        <v>password123</v>
-      </c>
-      <c r="C3" t="str">
-        <f>IF($C$2=Clients!$H3,Clients!H3,Clients!$H$4)</f>
-        <v>Active</v>
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>72</v>
@@ -1023,81 +1303,162 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
-        <f>IF($C$2=Clients!$H4,Clients!G4, Clients!G4)</f>
-        <v>janedoe</v>
-      </c>
-      <c r="B4" t="str">
-        <f>IF($C$2=Clients!$H4,Clients!C4, Clients!C4)</f>
-        <v>password123</v>
-      </c>
-      <c r="C4" t="str">
-        <f>IF($C$2=Clients!$H4,Clients!H4,Clients!$H$4)</f>
-        <v>Banned</v>
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
-        <f>IF($C$2=Clients!$H5,Clients!G5, Clients!G5)</f>
-        <v>bobsmith</v>
-      </c>
-      <c r="B5" t="str">
-        <f>IF($C$2=Clients!$H5,Clients!C5, Clients!C5)</f>
-        <v>password123</v>
-      </c>
-      <c r="C5" t="str">
-        <f>IF($C$2=Clients!$H5,Clients!H5,Clients!$H$4)</f>
-        <v>Active</v>
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E5" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
-        <f>IF($C$2=Clients!$H6,Clients!G6, Clients!G6)</f>
-        <v>alicejohnson</v>
-      </c>
-      <c r="B6" t="str">
-        <f>IF($C$2=Clients!$H6,Clients!C6, Clients!C6)</f>
-        <v>password123</v>
-      </c>
-      <c r="C6" t="str">
-        <f>IF($C$2=Clients!$H6,Clients!H6,Clients!$H$4)</f>
-        <v>Banned</v>
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>242</v>
+      </c>
+      <c r="E6" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="str" cm="1">
-        <f t="array" ref="A7">IF($C$2=Clients!$H7,Clients!G7, null)</f>
-        <v>mikebrown</v>
-      </c>
-      <c r="B7" t="str">
-        <f>IF($C$2=Clients!$H7,Clients!C7, Clients!C7)</f>
-        <v>password123</v>
-      </c>
-      <c r="C7" t="str">
-        <f>IF($C$2=Clients!$H7,Clients!H7,Clients!$H$4)</f>
-        <v>Active</v>
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>246</v>
+      </c>
+      <c r="E8" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>250</v>
+      </c>
+      <c r="E10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>252</v>
+      </c>
+      <c r="E11" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278CEAAF-5CBB-47DB-8AF0-25EE750EE6FA}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:R1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -1107,7 +1468,7 @@
     <col min="12" max="12" width="12.28515625" customWidth="1"/>
     <col min="13" max="13" width="7.5703125" customWidth="1"/>
     <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.42578125" customWidth="1"/>
+    <col min="15" max="15" width="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1157,9 +1518,56 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2">
+        <v>10001</v>
+      </c>
+      <c r="O2" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>18</v>
@@ -1168,37 +1576,37 @@
         <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="N3">
-        <v>10001</v>
+        <v>90001</v>
       </c>
       <c r="O3" t="s">
         <v>64</v>
@@ -1206,46 +1614,46 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="M4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N4">
-        <v>90001</v>
+        <v>80202</v>
       </c>
       <c r="O4" t="s">
         <v>64</v>
@@ -1253,46 +1661,46 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
         <v>23</v>
       </c>
       <c r="I5" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="J5" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="M5" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="N5">
-        <v>80202</v>
+        <v>60606</v>
       </c>
       <c r="O5" t="s">
         <v>64</v>
@@ -1300,95 +1708,236 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="I6" t="s">
         <v>67</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L6" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="M6" t="s">
         <v>69</v>
       </c>
       <c r="N6">
-        <v>60606</v>
+        <v>94105</v>
       </c>
       <c r="O6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>49</v>
+      <c r="A7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>63</v>
+      <c r="D7" s="2" t="s">
+        <v>255</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>168</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>169</v>
       </c>
       <c r="H7" t="s">
         <v>23</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>170</v>
       </c>
       <c r="J7" t="s">
-        <v>55</v>
+        <v>171</v>
       </c>
       <c r="K7" t="s">
-        <v>54</v>
+        <v>172</v>
       </c>
       <c r="L7" t="s">
-        <v>58</v>
+        <v>173</v>
       </c>
       <c r="M7" t="s">
-        <v>69</v>
+        <v>174</v>
       </c>
       <c r="N7">
-        <v>94105</v>
+        <v>2000</v>
       </c>
       <c r="O7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>177</v>
+      </c>
+      <c r="G8" t="s">
+        <v>178</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>179</v>
+      </c>
+      <c r="J8" t="s">
+        <v>180</v>
+      </c>
+      <c r="K8" t="s">
+        <v>181</v>
+      </c>
+      <c r="L8" t="s">
+        <v>179</v>
+      </c>
+      <c r="M8" t="s">
+        <v>182</v>
+      </c>
+      <c r="N8">
+        <v>18983</v>
+      </c>
+      <c r="O8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>187</v>
+      </c>
+      <c r="J9" t="s">
+        <v>188</v>
+      </c>
+      <c r="K9" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" t="s">
+        <v>189</v>
+      </c>
+      <c r="M9" t="s">
+        <v>190</v>
+      </c>
+      <c r="N9">
+        <v>75001</v>
+      </c>
+      <c r="O9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>259</v>
+      </c>
+      <c r="B10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" t="s">
+        <v>193</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>194</v>
+      </c>
+      <c r="J10" t="s">
+        <v>195</v>
+      </c>
+      <c r="K10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" t="s">
+        <v>196</v>
+      </c>
+      <c r="M10" t="s">
+        <v>197</v>
+      </c>
+      <c r="N10">
+        <v>10115</v>
+      </c>
+      <c r="O10" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1401,10 +1950,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69497AEC-9A82-4E0A-918B-D939B39B005B}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L1048576"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,154 +1993,299 @@
         <v>82</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="8" t="str">
+        <f>_xlfn.CONCAT(Clients!A2, " ",Clients!B2)</f>
+        <v>John Doe</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="B3" s="8" t="str">
         <f>_xlfn.CONCAT(Clients!A3, " ",Clients!B3)</f>
-        <v>John Doe</v>
+        <v>Jane Doe</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>134</v>
+        <v>130</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>103</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B4" s="8" t="str">
         <f>_xlfn.CONCAT(Clients!A4, " ",Clients!B4)</f>
-        <v>Jane Doe</v>
+        <v>Bob Smith</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B5" s="8" t="str">
         <f>_xlfn.CONCAT(Clients!A5, " ",Clients!B5)</f>
-        <v>Bob Smith</v>
+        <v>Alice Johnson</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>154</v>
+        <v>92</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B6" s="8" t="str">
         <f>_xlfn.CONCAT(Clients!A6, " ",Clients!B6)</f>
-        <v>Alice Johnson</v>
+        <v>Mike Brown</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" t="s">
+        <v>201</v>
+      </c>
+      <c r="G7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" t="s">
+        <v>205</v>
+      </c>
+      <c r="G8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" t="s">
+        <v>103</v>
+      </c>
+      <c r="I8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" t="s">
+        <v>209</v>
+      </c>
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D10" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="E10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" t="s">
+        <v>213</v>
+      </c>
+      <c r="G10" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H10" t="s">
         <v>103</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="8" t="str">
-        <f>_xlfn.CONCAT(Clients!A7, " ",Clients!B7)</f>
-        <v>Mike Brown</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="I10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D11" t="s">
         <v>153</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="E11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" t="s">
+        <v>217</v>
+      </c>
+      <c r="G11" t="s">
         <v>99</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H11" t="s">
         <v>104</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>100</v>
+      <c r="I11" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -1603,10 +2297,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE938AD-32A7-4EED-A9B8-EE1C285E7213}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="L1:M1048576"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,34 +2346,70 @@
         <v>84</v>
       </c>
     </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="5" t="str">
+        <f>(VLOOKUP(E2,Projects!A2:B6,2,1))</f>
+        <v>John Doe</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>145</v>
+        <v>108</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>149</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="I3" s="5" t="str">
-        <f>(VLOOKUP(E3,Projects!A3:B7,2,1))</f>
-        <v>John Doe</v>
+        <f>(VLOOKUP(E3,Projects!A3:B6,2,1))</f>
+        <v>Jane Doe</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>165</v>
@@ -1690,32 +2420,32 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>149</v>
+        <v>111</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>126</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I4" s="5" t="str">
-        <f>(VLOOKUP(E4,Projects!A4:B7,2,1))</f>
-        <v>Jane Doe</v>
+        <f>(VLOOKUP(E4,Projects!A4:B6,2,1))</f>
+        <v>Bob Smith</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>165</v>
@@ -1726,32 +2456,32 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>146</v>
+        <v>112</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="I5" s="5" t="str">
-        <f>(VLOOKUP(E5,Projects!A5:B7,2,1))</f>
-        <v>Bob Smith</v>
+        <f>(VLOOKUP(E5,Projects!A5:B6,2,1))</f>
+        <v>Alice Johnson</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>165</v>
@@ -1762,32 +2492,32 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>150</v>
+        <v>113</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="I6" s="5" t="str">
-        <f>(VLOOKUP(E6,Projects!A6:B7,2,1))</f>
-        <v>Alice Johnson</v>
+        <f>(VLOOKUP(E6,Projects!A2:B6,2,1))</f>
+        <v>Mike Brown</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>165</v>
@@ -1798,32 +2528,32 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>147</v>
+        <v>114</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="I7" s="5" t="str">
-        <f>(VLOOKUP(E7,Projects!A3:B7,2,1))</f>
-        <v>Mike Brown</v>
+        <f>(VLOOKUP(E7,Projects!A2:B6,2,1))</f>
+        <v>John Doe</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>165</v>
@@ -1834,32 +2564,32 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="I8" s="5" t="str">
-        <f>(VLOOKUP(E8,Projects!A3:B7,2,1))</f>
-        <v>John Doe</v>
+        <f>(VLOOKUP(E8,Projects!A3:B6,2,1))</f>
+        <v>Jane Doe</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>165</v>
@@ -1870,32 +2600,32 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="I9" s="5" t="str">
-        <f>(VLOOKUP(E9,Projects!A4:B7,2,1))</f>
-        <v>Jane Doe</v>
+        <f>(VLOOKUP(E9,Projects!A4:B6,2,1))</f>
+        <v>Mike Brown</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>165</v>
@@ -1905,38 +2635,142 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="I10" s="5" t="str">
-        <f>(VLOOKUP(E10,Projects!A5:B7,2,1))</f>
-        <v>Mike Brown</v>
+      <c r="A10" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>165</v>
       </c>
       <c r="K10" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>163</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Done All Flow Function Of Project
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginHRM.xlsx
+++ b/src/test/resources/testdata/LoginHRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Java\Project\FinalProjectAutomationTest\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F460FE-49E9-4E61-9813-4EE0D3DD1F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EAE841-DCFC-4913-B275-D374E7E57A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="4560" windowWidth="24120" windowHeight="11670" xr2:uid="{79BA1FD9-04F7-446D-A190-015AACA01288}"/>
+    <workbookView xWindow="4005" yWindow="4755" windowWidth="24120" windowHeight="10650" activeTab="2" xr2:uid="{79BA1FD9-04F7-446D-A190-015AACA01288}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="246">
   <si>
     <t>USERNAME</t>
   </si>
@@ -736,21 +736,6 @@
     <t>Database Design</t>
   </si>
   <si>
-    <t>Task 11</t>
-  </si>
-  <si>
-    <t>Apr, 2024, 10</t>
-  </si>
-  <si>
-    <t>Apr, 2024, 15</t>
-  </si>
-  <si>
-    <t>Task 12</t>
-  </si>
-  <si>
-    <t>May, 2024, 01</t>
-  </si>
-  <si>
     <t>JaneDoe1</t>
   </si>
   <si>
@@ -815,27 +800,6 @@
   </si>
   <si>
     <t>Kevin</t>
-  </si>
-  <si>
-    <t>TITLE_TASK</t>
-  </si>
-  <si>
-    <t>START_DATE_TASK</t>
-  </si>
-  <si>
-    <t>END_DATE_TASK</t>
-  </si>
-  <si>
-    <t>HOUR_TASK</t>
-  </si>
-  <si>
-    <t>SUMMARY_TASK</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_TASK</t>
-  </si>
-  <si>
-    <t>CLIENT_TASK</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367340E2-5DAD-4A3F-9862-8048D7AC0F7E}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B30:B31"/>
     </sheetView>
   </sheetViews>
@@ -1307,10 +1271,10 @@
         <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1324,10 +1288,10 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E5" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1341,10 +1305,10 @@
         <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E6" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,10 +1322,10 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E7" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1375,10 +1339,10 @@
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E8" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1392,10 +1356,10 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E9" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1409,10 +1373,10 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E10" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1426,10 +1390,10 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E11" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -1758,7 +1722,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E7" t="s">
         <v>29</v>
@@ -1805,7 +1769,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -1852,7 +1816,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -1890,7 +1854,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B10" t="s">
         <v>191</v>
@@ -1899,7 +1863,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
@@ -1946,8 +1910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69497AEC-9A82-4E0A-918B-D939B39B005B}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,7 +2110,7 @@
         <v>Emily Wilson</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D7" t="s">
         <v>86</v>
@@ -2296,10 +2260,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE938AD-32A7-4EED-A9B8-EE1C285E7213}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:N1048576"/>
+      <selection activeCell="L1" sqref="L1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,31 +2276,31 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>251</v>
+        <v>74</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>252</v>
+        <v>78</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>253</v>
+        <v>79</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>254</v>
+        <v>76</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>83</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>256</v>
+        <v>82</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>257</v>
+        <v>75</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>164</v>
@@ -2371,7 +2335,7 @@
         <v>107</v>
       </c>
       <c r="I2" s="5" t="str">
-        <f>(VLOOKUP(E2,Projects!A2:B6,2,1))</f>
+        <f>(VLOOKUP(E2,Projects!A2:B11,2,1))</f>
         <v>John Doe</v>
       </c>
       <c r="J2" s="5" t="s">
@@ -2407,7 +2371,7 @@
         <v>118</v>
       </c>
       <c r="I3" s="5" t="str">
-        <f>(VLOOKUP(E3,Projects!A3:B6,2,1))</f>
+        <f>(VLOOKUP(E3,Projects!A3:B7,2,1))</f>
         <v>Jane Doe</v>
       </c>
       <c r="J3" s="5" t="s">
@@ -2443,7 +2407,7 @@
         <v>120</v>
       </c>
       <c r="I4" s="5" t="str">
-        <f>(VLOOKUP(E4,Projects!A4:B6,2,1))</f>
+        <f>(VLOOKUP(E4,Projects!A4:B8,2,1))</f>
         <v>Bob Smith</v>
       </c>
       <c r="J4" s="5" t="s">
@@ -2479,7 +2443,7 @@
         <v>107</v>
       </c>
       <c r="I5" s="5" t="str">
-        <f>(VLOOKUP(E5,Projects!A5:B6,2,1))</f>
+        <f>(VLOOKUP(E5,Projects!A5:B9,2,1))</f>
         <v>Alice Johnson</v>
       </c>
       <c r="J5" s="5" t="s">
@@ -2515,7 +2479,7 @@
         <v>119</v>
       </c>
       <c r="I6" s="5" t="str">
-        <f>(VLOOKUP(E6,Projects!A2:B6,2,1))</f>
+        <f>(VLOOKUP(E6,Projects!A6:B10,2,1))</f>
         <v>Mike Brown</v>
       </c>
       <c r="J6" s="5" t="s">
@@ -2538,8 +2502,8 @@
       <c r="D7" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>85</v>
+      <c r="E7" t="s">
+        <v>198</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>160</v>
@@ -2551,8 +2515,8 @@
         <v>110</v>
       </c>
       <c r="I7" s="5" t="str">
-        <f>(VLOOKUP(E7,Projects!A2:B6,2,1))</f>
-        <v>John Doe</v>
+        <f>(VLOOKUP(E7,Projects!A7:B11,2,1))</f>
+        <v>Emily Wilson</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>165</v>
@@ -2574,8 +2538,8 @@
       <c r="D8" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>102</v>
+      <c r="E8" t="s">
+        <v>202</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>161</v>
@@ -2587,8 +2551,8 @@
         <v>119</v>
       </c>
       <c r="I8" s="5" t="str">
-        <f>(VLOOKUP(E8,Projects!A3:B6,2,1))</f>
-        <v>Jane Doe</v>
+        <f>(VLOOKUP(E8,Projects!A8:B11,2,1))</f>
+        <v>David Lee</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>165</v>
@@ -2610,8 +2574,8 @@
       <c r="D9" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>98</v>
+      <c r="E9" t="s">
+        <v>205</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>162</v>
@@ -2623,8 +2587,8 @@
         <v>110</v>
       </c>
       <c r="I9" s="5" t="str">
-        <f>(VLOOKUP(E9,Projects!A4:B6,2,1))</f>
-        <v>Mike Brown</v>
+        <f>(VLOOKUP(E9,Projects!A9:B11,2,1))</f>
+        <v>Sarah Taylor</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>165</v>
@@ -2646,8 +2610,8 @@
       <c r="D10" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>91</v>
+      <c r="E10" t="s">
+        <v>208</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>217</v>
@@ -2659,8 +2623,8 @@
         <v>107</v>
       </c>
       <c r="I10" s="5" t="str">
-        <f>(VLOOKUP(E10,Projects!A2:B11,2,1))</f>
-        <v>Bob Smith</v>
+        <f>(VLOOKUP(E10,Projects!A10:B11,2,1))</f>
+        <v>Kevin White</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>165</v>
@@ -2682,8 +2646,8 @@
       <c r="D11" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>95</v>
+      <c r="E11" t="s">
+        <v>211</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>222</v>
@@ -2695,85 +2659,13 @@
         <v>119</v>
       </c>
       <c r="I11" s="5" t="str">
-        <f>(VLOOKUP(E11,Projects!A3:B11,2,1))</f>
-        <v>Alice Johnson</v>
+        <f>(VLOOKUP(E11,Projects!A11:B11,2,1))</f>
+        <v>Mike Brown</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>165</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I12" s="5" t="str">
-        <f>(VLOOKUP(E12,Projects!A4:B11,2,1))</f>
-        <v>Mike Brown</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="I13" s="5" t="str">
-        <f>(VLOOKUP(E13,Projects!A2:B11,2,1))</f>
-        <v>John Doe</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="K13" s="5" t="s">
         <v>163</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix function initData pagekage
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginHRM.xlsx
+++ b/src/test/resources/testdata/LoginHRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Java\Project\FinalProjectAutomationTest\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EAE841-DCFC-4913-B275-D374E7E57A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B31F0F-6F7B-4667-B0D7-EA29036039A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="4755" windowWidth="24120" windowHeight="10650" activeTab="2" xr2:uid="{79BA1FD9-04F7-446D-A190-015AACA01288}"/>
+    <workbookView xWindow="2640" yWindow="3870" windowWidth="24120" windowHeight="10020" activeTab="1" xr2:uid="{79BA1FD9-04F7-446D-A190-015AACA01288}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278CEAAF-5CBB-47DB-8AF0-25EE750EE6FA}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1910,7 +1910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69497AEC-9A82-4E0A-918B-D939B39B005B}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>